<commit_message>
update of GL for face images
</commit_message>
<xml_diff>
--- a/single_digit/Results/3vs5_CNN_GL.xlsx
+++ b/single_digit/Results/3vs5_CNN_GL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\Group_Learning\single_digit\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AAD379-082E-4375-A7DB-F96F972E569D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0E3485-D5C7-4790-A06E-3905025AF131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0A4D5629-DDC9-4A37-80E7-A4A435BAA222}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0A4D5629-DDC9-4A37-80E7-A4A435BAA222}"/>
   </bookViews>
   <sheets>
     <sheet name="CNN" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
   <si>
     <t xml:space="preserve">window </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -58,6 +58,14 @@
   </si>
   <si>
     <t>MEAN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -350,19 +358,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.31029999999999996</c:v>
+                  <c:v>0.2104</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.31029999999999996</c:v>
+                  <c:v>0.2104</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.31029999999999996</c:v>
+                  <c:v>0.2104</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.31029999999999996</c:v>
+                  <c:v>0.2104</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.31029999999999996</c:v>
+                  <c:v>0.2104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -919,19 +927,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.02</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.02</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.02</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.02</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.02</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2768,66 +2776,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82751D7-CEC9-4A47-9053-B670E3828681}">
-  <dimension ref="A2:J27"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
   <sheetData>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
+    <row r="1" spans="2:10">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="2" spans="2:10">
+      <c r="B2">
+        <v>0.23</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10">
       <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>0.182</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
       <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>0.185</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
       <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
       <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
       <c r="B7">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
       <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>0.252</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
       <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>0.248</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
       <c r="B10">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
       <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
       <c r="B12">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="C12">
         <v>0</v>
       </c>
       <c r="F12">
@@ -2846,115 +2895,132 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="2:10">
       <c r="B13">
-        <f>AVERAGE(B3:B12)</f>
-        <v>0.02</v>
+        <v>0.246</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>0.31029999999999996</v>
+        <v>0.2104</v>
       </c>
       <c r="G13">
-        <v>0.31029999999999996</v>
+        <v>0.2104</v>
       </c>
       <c r="H13">
-        <v>0.31029999999999996</v>
+        <v>0.2104</v>
       </c>
       <c r="I13">
-        <v>0.31029999999999996</v>
+        <v>0.2104</v>
       </c>
       <c r="J13">
-        <v>0.31029999999999996</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>0.2104</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14">
+        <v>0.21</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
       <c r="F14">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="J14">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15">
+        <v>0.188</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
       <c r="B16">
-        <v>0.30399999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="B17">
-        <v>0.29399999999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>0.214</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="B18">
-        <v>0.377</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>0.22</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="B19">
-        <v>0.27300000000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="B20">
-        <v>0.32600000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="B21">
-        <v>0.27300000000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
       <c r="B22">
-        <v>0.34399999999999997</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <f>AVERAGE(B2:B21)</f>
+        <v>0.2104</v>
+      </c>
+      <c r="C22">
+        <f>AVERAGE(C2:C21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
       <c r="B23">
-        <v>0.33700000000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="B24">
-        <v>0.26300000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="B25">
-        <v>0.312</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26">
-        <f>AVERAGE(B16:B25)</f>
-        <v>0.31029999999999996</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27">
-        <f>STDEV(B16:B25)</f>
-        <v>3.6319722221160061E-2</v>
+        <f>STDEV(B2:B21)</f>
+        <v>2.5411145503291897E-2</v>
+      </c>
+      <c r="C23">
+        <f>STDEV(C2:C21)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2968,7 +3034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C06305DA-4BBB-4C2F-9010-8C6B7BDC7A27}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -3458,8 +3524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A669EFFF-3957-4635-94B0-01F3A9B99E19}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="V23" sqref="V23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>

</xml_diff>